<commit_message>
added tools size, semi complete
</commit_message>
<xml_diff>
--- a/ScreenTree.xlsx
+++ b/ScreenTree.xlsx
@@ -36,9 +36,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
     <t>GLM</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>Random Forest (RF)</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -547,7 +547,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -555,10 +555,10 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -566,17 +566,17 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -584,10 +584,10 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -595,10 +595,10 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -626,20 +626,20 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -653,7 +653,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -661,10 +661,10 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -672,7 +672,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -680,10 +680,10 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -691,10 +691,10 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="E19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -702,7 +702,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -710,10 +710,10 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="E21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -721,17 +721,17 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="E22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -739,7 +739,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="2"/>
     </row>
@@ -748,13 +748,13 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -763,10 +763,10 @@
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -781,7 +781,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" s="2"/>
     </row>
@@ -791,10 +791,10 @@
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -803,10 +803,10 @@
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:6">

</xml_diff>